<commit_message>
Update EXSIM_Mezquite_Purchasing_CORREGIDO_FIX_with_policies.xlsx to incorporate necessary policy adjustments
</commit_message>
<xml_diff>
--- a/Marketing/ForecastOutput.xlsx
+++ b/Marketing/ForecastOutput.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0dc407a335d7300f/Documentos/GitHub/BusinessSim/Marketing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{9D71A1DC-30E0-4944-9368-052DCF0EDF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7397D477-7F39-455A-9F6C-663F3611141E}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{9D71A1DC-30E0-4944-9368-052DCF0EDF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D899DBD1-F3B6-4653-B944-BB8731D1A0F2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD248430-E1E1-4301-A005-AFE5B8A20DF6}"/>
   </bookViews>
   <sheets>
     <sheet name="ForecastOutput" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="39">
   <si>
     <t>Region</t>
   </si>
@@ -134,12 +147,18 @@
   </si>
   <si>
     <t>por periodo</t>
+  </si>
+  <si>
+    <t>Columna1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -573,7 +592,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -616,12 +635,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -654,6 +675,7 @@
     <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Moneda" xfId="42" builtinId="4"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
@@ -676,6 +698,36 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E2E54D6-0C6E-41CE-96A6-82D6407B52C3}" name="Tabla1" displayName="Tabla1" ref="A1:I21" totalsRowShown="0">
+  <autoFilter ref="A1:I21" xr:uid="{2E2E54D6-0C6E-41CE-96A6-82D6407B52C3}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="9"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{497CDC21-2362-4948-907E-F29A27EFA145}" name="Region"/>
+    <tableColumn id="2" xr3:uid="{C3488C69-6D66-4132-94E9-A7C88B527A63}" name="Model"/>
+    <tableColumn id="3" xr3:uid="{9D78044A-A094-408F-89F3-D7A672C6AF63}" name="Period"/>
+    <tableColumn id="4" xr3:uid="{FA41B3A6-6685-4788-AA86-530B6C5D0EA7}" name="Season"/>
+    <tableColumn id="5" xr3:uid="{37863176-1944-4D07-BB7B-3735C15C6D08}" name="Forecast_Sales"/>
+    <tableColumn id="6" xr3:uid="{FD8C1791-2C8E-4D43-86C8-A6509E7522C7}" name="ColdStart_Forecast"/>
+    <tableColumn id="7" xr3:uid="{08AC0726-044E-4FEA-A328-6555272A568B}" name="Forecast_Sales_Final"/>
+    <tableColumn id="8" xr3:uid="{74CDCECD-5236-4EA3-8597-9714A52814E0}" name="Columna1"/>
+    <tableColumn id="9" xr3:uid="{7C59A30C-9CDC-41B7-9EFA-E796268ABC50}" name="Our sales">
+      <calculatedColumnFormula>G2*0.14</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -995,13 +1047,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F40A51E8-42EB-40C8-A800-E58BFD210842}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="18.21875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1025,6 +1084,9 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
       <c r="I1" t="s">
         <v>36</v>
       </c>
@@ -1053,7 +1115,7 @@
         <v>9981.1406090440396</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1077,7 +1139,7 @@
         <v>8752.6411926338569</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1101,7 +1163,7 @@
         <v>6795.9551681088205</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1149,7 +1211,7 @@
         <v>1606.454304950292</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1173,7 +1235,7 @@
         <v>2241.8756230541721</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1197,7 +1259,7 @@
         <v>2154.9415285602122</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1245,7 +1307,7 @@
         <v>5627.855111690239</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1269,7 +1331,7 @@
         <v>5608.1353845549902</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1293,7 +1355,7 @@
         <v>6138.4101742087178</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1341,7 +1403,7 @@
         <v>1188.5166222309676</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1365,7 +1427,7 @@
         <v>1658.625729199754</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1389,7 +1451,7 @@
         <v>1594.3085456818242</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -1413,7 +1475,7 @@
         <v>2156.9870864500281</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1437,7 +1499,7 @@
         <v>4932.676803673934</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1461,7 +1523,7 @@
         <v>5115.6086475315651</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1485,7 +1547,7 @@
         <v>5373.8597520091816</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -1509,13 +1571,13 @@
         <v>6081.6300574052811</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="I22">
         <f>+SUM(I2:I21)</f>
         <v>98842.781646401068</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H24" t="s">
         <v>37</v>
       </c>
@@ -1523,8 +1585,44 @@
         <f>+I22/4</f>
         <v>24710.695411600267</v>
       </c>
+      <c r="R24">
+        <v>23384</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K25" s="2">
+        <f>+I2+I6+I10+I14+I18</f>
+        <v>23336.643451589473</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="N26">
+        <f>22500*0.8</f>
+        <v>18000</v>
+      </c>
+      <c r="O26">
+        <f>+N26*1.2</f>
+        <v>21600</v>
+      </c>
+      <c r="R26">
+        <f>+R24/1.2</f>
+        <v>19486.666666666668</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="N28">
+        <f>22500/1.2</f>
+        <v>18750</v>
+      </c>
+      <c r="O28">
+        <f>+N28*1.2</f>
+        <v>22500</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>